<commit_message>
Upload and presentation done
</commit_message>
<xml_diff>
--- a/Documentation/Calculations.xlsx
+++ b/Documentation/Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anszilas\Documents\GitHub\HEKK\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5BE70C-3940-4F0C-92EF-F5AD437564D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CAA8BD-517F-4169-99D8-3A3BAE77E599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ControllerBox price" sheetId="3" r:id="rId1"/>
@@ -1519,7 +1519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75181827-F6C5-4D7F-B565-B46DFA857A5C}">
   <dimension ref="B2:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1647,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45619176-1AAB-4F2A-9925-3C8F3A8DD104}">
   <dimension ref="B3:I21"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1676,7 +1676,7 @@
         <v>39</v>
       </c>
       <c r="I3">
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
@@ -1715,7 +1715,7 @@
         <v>36</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>41</v>
@@ -1730,7 +1730,7 @@
       </c>
       <c r="C9">
         <f>C5-C6</f>
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
@@ -1757,7 +1757,7 @@
       </c>
       <c r="C12">
         <f>C11*C9*F3</f>
-        <v>3034.5840000000003</v>
+        <v>2528.8200000000002</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="C13">
         <f>C12/(3600*I6)</f>
-        <v>1.6858800000000003</v>
+        <v>1.4049</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
@@ -1775,7 +1775,7 @@
       </c>
       <c r="C14">
         <f>C13/1000 * I3</f>
-        <v>0.5057640000000001</v>
+        <v>0.35122500000000001</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
@@ -1784,7 +1784,7 @@
       </c>
       <c r="C15">
         <f>C14*I5</f>
-        <v>212.42088000000004</v>
+        <v>147.5145</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
@@ -1793,13 +1793,13 @@
       </c>
       <c r="C17" s="2">
         <f>C15*90*F17</f>
-        <v>24853.242960000003</v>
+        <v>19914.4575</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>50</v>
       </c>
       <c r="F17">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
@@ -1808,7 +1808,7 @@
       </c>
       <c r="C18" s="4">
         <f>C17/I5</f>
-        <v>59.174388000000008</v>
+        <v>47.415375000000004</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
@@ -1817,7 +1817,7 @@
       </c>
       <c r="C20" s="2">
         <f>C17*1.5</f>
-        <v>37279.864440000005</v>
+        <v>29871.686249999999</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
@@ -1826,7 +1826,7 @@
       </c>
       <c r="C21" s="4">
         <f>C18*1.5</f>
-        <v>88.761582000000004</v>
+        <v>71.123062500000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>